<commit_message>
unnecessary id_scenario columns removed from tables
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_UnitUser.xlsx
+++ b/projects/test_building/input/Scenario_UnitUser.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D97374-907B-6447-AF6A-72396AF5A139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2B4652-6A31-1645-BBCD-1D1F40A1836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4600" yWindow="760" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
-  <si>
-    <t>id_scenario</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>unit</t>
   </si>
@@ -181,10 +178,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Q9" totalsRowShown="0">
-  <autoFilter ref="A1:Q9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_scenario"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P9" totalsRowShown="0">
+  <autoFilter ref="A1:P9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="16">
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="id_region"/>
     <tableColumn id="7" xr3:uid="{8D3F057E-E79A-644F-B285-449A127EBD2A}" name="id_sector"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="id_unit_user_type"/>
@@ -469,37 +465,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="13" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
-      </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -523,37 +518,32 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="N1" t="s">
         <v>2</v>
       </c>
       <c r="O1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -561,30 +551,27 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1">
+      <c r="M2" s="1">
         <v>0.19676806083650186</v>
       </c>
+      <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -592,30 +579,27 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1">
+      <c r="M3" s="1">
         <v>0.20532319391634976</v>
       </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -623,30 +607,27 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1">
+      <c r="M4" s="1">
         <v>0.16634980988593154</v>
       </c>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -654,30 +635,27 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1">
+      <c r="M5" s="1">
         <v>0.20247148288973379</v>
       </c>
+      <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
         <v>5</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -685,30 +663,27 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1">
+      <c r="M6" s="1">
         <v>8.1749049429657786E-2</v>
       </c>
+      <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -716,30 +691,27 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1">
+      <c r="M7" s="1">
         <v>9.8859315589353611E-2</v>
       </c>
+      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -747,30 +719,27 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1">
+      <c r="M8" s="1">
         <v>4.8479087452471474E-2</v>
       </c>
+      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
         <v>8</v>
       </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -778,13 +747,12 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1">
+      <c r="M9" s="1">
         <v>1</v>
       </c>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>